<commit_message>
adding power bi stuff
</commit_message>
<xml_diff>
--- a/Finance Database.xlsx
+++ b/Finance Database.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Expense</t>
   </si>
@@ -52,156 +52,226 @@
     <t>Savings</t>
   </si>
   <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Mutual funds</t>
+  </si>
+  <si>
+    <t>EMIs</t>
+  </si>
+  <si>
+    <t>House Rent</t>
+  </si>
+  <si>
+    <t>Groceries &amp; Food</t>
+  </si>
+  <si>
+    <t>Jan-18</t>
+  </si>
+  <si>
+    <t>Feb-18</t>
+  </si>
+  <si>
+    <t>Mar-18</t>
+  </si>
+  <si>
+    <t>Apr-18</t>
+  </si>
+  <si>
+    <t>May-18</t>
+  </si>
+  <si>
+    <t>Jun-18</t>
+  </si>
+  <si>
+    <t>Jul-18</t>
+  </si>
+  <si>
+    <t>Aug-18</t>
+  </si>
+  <si>
+    <t>Sep-18</t>
+  </si>
+  <si>
+    <t>Oct-18</t>
+  </si>
+  <si>
+    <t>Nov-18</t>
+  </si>
+  <si>
+    <t>Dec-18</t>
+  </si>
+  <si>
+    <t>Jan-19</t>
+  </si>
+  <si>
+    <t>Feb-19</t>
+  </si>
+  <si>
+    <t>Mar-19</t>
+  </si>
+  <si>
+    <t>Apr-19</t>
+  </si>
+  <si>
+    <t>May-19</t>
+  </si>
+  <si>
+    <t>Jun-19</t>
+  </si>
+  <si>
+    <t>Jul-19</t>
+  </si>
+  <si>
+    <t>Aug-19</t>
+  </si>
+  <si>
+    <t>Sep-19</t>
+  </si>
+  <si>
+    <t>Oct-19</t>
+  </si>
+  <si>
+    <t>Nov-19</t>
+  </si>
+  <si>
+    <t>Dec-19</t>
+  </si>
+  <si>
+    <t>Jan-20</t>
+  </si>
+  <si>
+    <t>Feb-20</t>
+  </si>
+  <si>
+    <t>Mar-20</t>
+  </si>
+  <si>
+    <t>Apr-20</t>
+  </si>
+  <si>
+    <t>May-20</t>
+  </si>
+  <si>
+    <t>Jun-20</t>
+  </si>
+  <si>
+    <t>Jul-20</t>
+  </si>
+  <si>
+    <t>Aug-20</t>
+  </si>
+  <si>
+    <t>Sep-20</t>
+  </si>
+  <si>
+    <t>Oct-20</t>
+  </si>
+  <si>
+    <t>Nov-20</t>
+  </si>
+  <si>
+    <t>Dec-20</t>
+  </si>
+  <si>
+    <t>Jan-21</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Feb-22</t>
+  </si>
+  <si>
+    <t>Mar-22</t>
+  </si>
+  <si>
+    <t>Apr-22</t>
+  </si>
+  <si>
+    <t>May-22</t>
+  </si>
+  <si>
+    <t>Jun-22</t>
+  </si>
+  <si>
+    <t>Feb-21</t>
+  </si>
+  <si>
+    <t>Mar-21</t>
+  </si>
+  <si>
+    <t>Apr-21</t>
+  </si>
+  <si>
+    <t>May-21</t>
+  </si>
+  <si>
+    <t>Jun-21</t>
+  </si>
+  <si>
+    <t>Jul-21</t>
+  </si>
+  <si>
+    <t>Aug-21</t>
+  </si>
+  <si>
+    <t>Sep-21</t>
+  </si>
+  <si>
+    <t>Oct-21</t>
+  </si>
+  <si>
+    <t>Nov-21</t>
+  </si>
+  <si>
+    <t>Dec-21</t>
+  </si>
+  <si>
+    <t>Jan-22</t>
+  </si>
+  <si>
+    <t>Jul-22</t>
+  </si>
+  <si>
+    <t>Aug-22</t>
+  </si>
+  <si>
+    <t>Sep-22</t>
+  </si>
+  <si>
+    <t>Oct-22</t>
+  </si>
+  <si>
+    <t>Nov-22</t>
+  </si>
+  <si>
+    <t>Dec-22</t>
+  </si>
+  <si>
+    <t>Emergency Fund</t>
+  </si>
+  <si>
+    <t>Fixed Deposit</t>
+  </si>
+  <si>
+    <t>Liquid Cash</t>
+  </si>
+  <si>
     <t>Health</t>
   </si>
   <si>
-    <t>Component</t>
-  </si>
-  <si>
     <t>Leisure</t>
-  </si>
-  <si>
-    <t>Emergency Fund</t>
-  </si>
-  <si>
-    <t>Mutual funds</t>
-  </si>
-  <si>
-    <t>Fixed Deposit</t>
-  </si>
-  <si>
-    <t>EMIs</t>
-  </si>
-  <si>
-    <t>House Rent</t>
-  </si>
-  <si>
-    <t>Liquid Cash</t>
-  </si>
-  <si>
-    <t>Groceries &amp; Food</t>
-  </si>
-  <si>
-    <t>Jan-18</t>
-  </si>
-  <si>
-    <t>Feb-18</t>
-  </si>
-  <si>
-    <t>Mar-18</t>
-  </si>
-  <si>
-    <t>Apr-18</t>
-  </si>
-  <si>
-    <t>May-18</t>
-  </si>
-  <si>
-    <t>Jun-18</t>
-  </si>
-  <si>
-    <t>Jul-18</t>
-  </si>
-  <si>
-    <t>Aug-18</t>
-  </si>
-  <si>
-    <t>Sep-18</t>
-  </si>
-  <si>
-    <t>Oct-18</t>
-  </si>
-  <si>
-    <t>Nov-18</t>
-  </si>
-  <si>
-    <t>Dec-18</t>
-  </si>
-  <si>
-    <t>Jan-19</t>
-  </si>
-  <si>
-    <t>Feb-19</t>
-  </si>
-  <si>
-    <t>Mar-19</t>
-  </si>
-  <si>
-    <t>Apr-19</t>
-  </si>
-  <si>
-    <t>May-19</t>
-  </si>
-  <si>
-    <t>Jun-19</t>
-  </si>
-  <si>
-    <t>Jul-19</t>
-  </si>
-  <si>
-    <t>Aug-19</t>
-  </si>
-  <si>
-    <t>Sep-19</t>
-  </si>
-  <si>
-    <t>Oct-19</t>
-  </si>
-  <si>
-    <t>Nov-19</t>
-  </si>
-  <si>
-    <t>Dec-19</t>
-  </si>
-  <si>
-    <t>Jan-20</t>
-  </si>
-  <si>
-    <t>Feb-20</t>
-  </si>
-  <si>
-    <t>Mar-20</t>
-  </si>
-  <si>
-    <t>Apr-20</t>
-  </si>
-  <si>
-    <t>May-20</t>
-  </si>
-  <si>
-    <t>Jun-20</t>
-  </si>
-  <si>
-    <t>Jul-20</t>
-  </si>
-  <si>
-    <t>Aug-20</t>
-  </si>
-  <si>
-    <t>Sep-20</t>
-  </si>
-  <si>
-    <t>Oct-20</t>
-  </si>
-  <si>
-    <t>Nov-20</t>
-  </si>
-  <si>
-    <t>Dec-20</t>
-  </si>
-  <si>
-    <t>Jan-21</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    <numFmt numFmtId="165" formatCode="mmm\-yy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -238,16 +308,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="61">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$₹-439]#,##0"/>
     </dxf>
@@ -376,48 +516,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FinData" displayName="FinData" ref="A2:AM14" totalsRowShown="0" headerRowDxfId="37">
-  <autoFilter ref="A2:AM14"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FinData" displayName="FinData" ref="A2:BJ14" totalsRowShown="0" headerRowDxfId="60">
+  <autoFilter ref="A2:BJ14"/>
+  <tableColumns count="62">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Component"/>
-    <tableColumn id="3" name="Jan-18" dataDxfId="36"/>
-    <tableColumn id="4" name="Feb-18" dataDxfId="35"/>
-    <tableColumn id="5" name="Mar-18" dataDxfId="34"/>
-    <tableColumn id="6" name="Apr-18" dataDxfId="33"/>
-    <tableColumn id="7" name="May-18" dataDxfId="32"/>
-    <tableColumn id="8" name="Jun-18" dataDxfId="31"/>
-    <tableColumn id="9" name="Jul-18" dataDxfId="30"/>
-    <tableColumn id="10" name="Aug-18" dataDxfId="29"/>
-    <tableColumn id="11" name="Sep-18" dataDxfId="28"/>
-    <tableColumn id="12" name="Oct-18" dataDxfId="27"/>
-    <tableColumn id="13" name="Nov-18" dataDxfId="26"/>
-    <tableColumn id="14" name="Dec-18" dataDxfId="25"/>
-    <tableColumn id="15" name="Jan-19" dataDxfId="24"/>
-    <tableColumn id="16" name="Feb-19" dataDxfId="23"/>
-    <tableColumn id="17" name="Mar-19" dataDxfId="22"/>
-    <tableColumn id="18" name="Apr-19" dataDxfId="21"/>
-    <tableColumn id="19" name="May-19" dataDxfId="20"/>
-    <tableColumn id="20" name="Jun-19" dataDxfId="19"/>
-    <tableColumn id="21" name="Jul-19" dataDxfId="18"/>
-    <tableColumn id="22" name="Aug-19" dataDxfId="1"/>
-    <tableColumn id="23" name="Sep-19" dataDxfId="2"/>
-    <tableColumn id="24" name="Oct-19" dataDxfId="0"/>
-    <tableColumn id="25" name="Nov-19" dataDxfId="17"/>
-    <tableColumn id="26" name="Dec-19" dataDxfId="16"/>
-    <tableColumn id="27" name="Jan-20" dataDxfId="15"/>
-    <tableColumn id="28" name="Feb-20" dataDxfId="14"/>
-    <tableColumn id="29" name="Mar-20" dataDxfId="13"/>
-    <tableColumn id="30" name="Apr-20" dataDxfId="12"/>
-    <tableColumn id="31" name="May-20" dataDxfId="11"/>
-    <tableColumn id="32" name="Jun-20" dataDxfId="10"/>
-    <tableColumn id="33" name="Jul-20" dataDxfId="9"/>
-    <tableColumn id="34" name="Aug-20" dataDxfId="8"/>
-    <tableColumn id="35" name="Sep-20" dataDxfId="7"/>
-    <tableColumn id="36" name="Oct-20" dataDxfId="6"/>
-    <tableColumn id="37" name="Nov-20" dataDxfId="5"/>
-    <tableColumn id="38" name="Dec-20" dataDxfId="4"/>
-    <tableColumn id="39" name="Jan-21" dataDxfId="3"/>
+    <tableColumn id="3" name="Jan-18" dataDxfId="59"/>
+    <tableColumn id="4" name="Feb-18" dataDxfId="58"/>
+    <tableColumn id="5" name="Mar-18" dataDxfId="57"/>
+    <tableColumn id="6" name="Apr-18" dataDxfId="56"/>
+    <tableColumn id="7" name="May-18" dataDxfId="55"/>
+    <tableColumn id="8" name="Jun-18" dataDxfId="54"/>
+    <tableColumn id="9" name="Jul-18" dataDxfId="53"/>
+    <tableColumn id="10" name="Aug-18" dataDxfId="52"/>
+    <tableColumn id="11" name="Sep-18" dataDxfId="51"/>
+    <tableColumn id="12" name="Oct-18" dataDxfId="50"/>
+    <tableColumn id="13" name="Nov-18" dataDxfId="49"/>
+    <tableColumn id="14" name="Dec-18" dataDxfId="48"/>
+    <tableColumn id="15" name="Jan-19" dataDxfId="47"/>
+    <tableColumn id="16" name="Feb-19" dataDxfId="46"/>
+    <tableColumn id="17" name="Mar-19" dataDxfId="45"/>
+    <tableColumn id="18" name="Apr-19" dataDxfId="44"/>
+    <tableColumn id="19" name="May-19" dataDxfId="43"/>
+    <tableColumn id="20" name="Jun-19" dataDxfId="42"/>
+    <tableColumn id="21" name="Jul-19" dataDxfId="41"/>
+    <tableColumn id="22" name="Aug-19" dataDxfId="40"/>
+    <tableColumn id="23" name="Sep-19" dataDxfId="39"/>
+    <tableColumn id="24" name="Oct-19" dataDxfId="38"/>
+    <tableColumn id="25" name="Nov-19" dataDxfId="37"/>
+    <tableColumn id="26" name="Dec-19" dataDxfId="36"/>
+    <tableColumn id="27" name="Jan-20" dataDxfId="35"/>
+    <tableColumn id="28" name="Feb-20" dataDxfId="34"/>
+    <tableColumn id="29" name="Mar-20" dataDxfId="33"/>
+    <tableColumn id="30" name="Apr-20" dataDxfId="32"/>
+    <tableColumn id="31" name="May-20" dataDxfId="31"/>
+    <tableColumn id="32" name="Jun-20" dataDxfId="30"/>
+    <tableColumn id="33" name="Jul-20" dataDxfId="29"/>
+    <tableColumn id="34" name="Aug-20" dataDxfId="28"/>
+    <tableColumn id="35" name="Sep-20" dataDxfId="27"/>
+    <tableColumn id="36" name="Oct-20" dataDxfId="26"/>
+    <tableColumn id="37" name="Nov-20" dataDxfId="25"/>
+    <tableColumn id="38" name="Dec-20" dataDxfId="24"/>
+    <tableColumn id="39" name="Jan-21" dataDxfId="23"/>
+    <tableColumn id="40" name="Feb-21" dataDxfId="22"/>
+    <tableColumn id="41" name="Mar-21" dataDxfId="21"/>
+    <tableColumn id="42" name="Apr-21" dataDxfId="20"/>
+    <tableColumn id="43" name="May-21" dataDxfId="19"/>
+    <tableColumn id="44" name="Jun-21" dataDxfId="18"/>
+    <tableColumn id="45" name="Jul-21" dataDxfId="17"/>
+    <tableColumn id="46" name="Aug-21" dataDxfId="16"/>
+    <tableColumn id="47" name="Sep-21" dataDxfId="15"/>
+    <tableColumn id="48" name="Oct-21" dataDxfId="14"/>
+    <tableColumn id="49" name="Nov-21" dataDxfId="13"/>
+    <tableColumn id="50" name="Dec-21" dataDxfId="12"/>
+    <tableColumn id="51" name="Jan-22" dataDxfId="11"/>
+    <tableColumn id="52" name="Feb-22" dataDxfId="10"/>
+    <tableColumn id="53" name="Mar-22" dataDxfId="9"/>
+    <tableColumn id="54" name="Apr-22" dataDxfId="8"/>
+    <tableColumn id="55" name="May-22" dataDxfId="7"/>
+    <tableColumn id="56" name="Jun-22" dataDxfId="6"/>
+    <tableColumn id="57" name="Jul-22" dataDxfId="5"/>
+    <tableColumn id="58" name="Aug-22" dataDxfId="4"/>
+    <tableColumn id="59" name="Sep-22" dataDxfId="3"/>
+    <tableColumn id="60" name="Oct-22" dataDxfId="2"/>
+    <tableColumn id="61" name="Nov-22" dataDxfId="1"/>
+    <tableColumn id="62" name="Dec-22" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -720,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AT14"/>
+  <dimension ref="A2:BJ14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,136 +894,200 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="39" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="35" width="10.5703125" customWidth="1"/>
+    <col min="36" max="36" width="7.85546875" customWidth="1"/>
+    <col min="37" max="39" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
+      <c r="BE2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -978,8 +1205,77 @@
       <c r="AM3" s="2">
         <v>51500</v>
       </c>
+      <c r="AN3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="AV3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AW3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AX3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AY3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="AZ3" s="2">
+        <v>43000</v>
+      </c>
+      <c r="BA3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BB3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BC3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BD3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BE3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BF3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BG3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BH3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>51500</v>
+      </c>
+      <c r="BJ3" s="2">
+        <v>51500</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1097,13 +1393,82 @@
       <c r="AM4" s="2">
         <v>6000</v>
       </c>
+      <c r="AN4" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AO4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AS4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AT4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AU4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AV4" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AW4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AX4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AY4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="AZ4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BA4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BB4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BC4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BD4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BE4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BF4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BG4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BH4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BI4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="BJ4" s="2">
+        <v>6000</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>5000</v>
@@ -1216,13 +1581,82 @@
       <c r="AM5" s="2">
         <v>8000</v>
       </c>
+      <c r="AN5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AP5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AQ5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AW5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AX5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AY5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="AZ5" s="2">
+        <v>7000</v>
+      </c>
+      <c r="BA5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BB5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BC5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BD5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BE5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BF5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BG5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BH5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BI5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BJ5" s="2">
+        <v>8000</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2">
         <v>2000</v>
@@ -1335,13 +1769,82 @@
       <c r="AM6" s="2">
         <v>3000</v>
       </c>
+      <c r="AN6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AV6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AX6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AY6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AZ6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BB6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BC6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BD6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BF6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BG6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BH6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="BI6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BJ6" s="2">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2">
         <v>2000</v>
@@ -1454,13 +1957,82 @@
       <c r="AM7" s="2">
         <v>2500</v>
       </c>
+      <c r="AN7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="AV7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AW7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AZ7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BB7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BC7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BD7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BE7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BF7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BG7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BH7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BI7" s="2">
+        <v>2500</v>
+      </c>
+      <c r="BJ7" s="2">
+        <v>2500</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2">
         <f>SUM(C3:C4)-SUM(C5:C7)-SUM(C9:C14)</f>
@@ -1610,13 +2182,105 @@
         <f t="shared" si="0"/>
         <v>-500</v>
       </c>
+      <c r="AN8" s="2">
+        <f t="shared" ref="AN8:BK8" si="1">SUM(AN3:AN4)-SUM(AN5:AN7)-SUM(AN9:AN14)</f>
+        <v>1500</v>
+      </c>
+      <c r="AO8" s="2">
+        <f t="shared" si="1"/>
+        <v>-1500</v>
+      </c>
+      <c r="AP8" s="2">
+        <f t="shared" si="1"/>
+        <v>-2000</v>
+      </c>
+      <c r="AQ8" s="2">
+        <f t="shared" si="1"/>
+        <v>-2500</v>
+      </c>
+      <c r="AR8" s="2">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="AS8" s="2">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="AT8" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="AU8" s="2">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="AV8" s="2">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="AW8" s="2">
+        <f t="shared" si="1"/>
+        <v>-1500</v>
+      </c>
+      <c r="AX8" s="2">
+        <f t="shared" si="1"/>
+        <v>-2000</v>
+      </c>
+      <c r="AY8" s="2">
+        <f t="shared" si="1"/>
+        <v>-2500</v>
+      </c>
+      <c r="AZ8" s="2">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="BA8" s="2">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="BB8" s="2">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="BC8" s="2">
+        <f t="shared" si="1"/>
+        <v>-500</v>
+      </c>
+      <c r="BD8" s="2">
+        <f t="shared" ref="BD8:BI8" si="2">SUM(BD3:BD4)-SUM(BD5:BD7)-SUM(BD9:BD14)</f>
+        <v>1500</v>
+      </c>
+      <c r="BE8" s="2">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="BF8" s="2">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="BG8" s="2">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+      <c r="BH8" s="2">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="BI8" s="2">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="BJ8" s="2">
+        <f t="shared" ref="BJ8" si="3">SUM(BJ3:BJ4)-SUM(BJ5:BJ7)-SUM(BJ9:BJ14)</f>
+        <v>-500</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>10000</v>
@@ -1729,13 +2393,82 @@
       <c r="AM9" s="2">
         <v>16000</v>
       </c>
+      <c r="AN9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AQ9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AR9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AS9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AT9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AU9" s="2">
+        <v>16000</v>
+      </c>
+      <c r="AV9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AW9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AX9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AY9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AZ9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BA9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BB9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BC9" s="2">
+        <v>16000</v>
+      </c>
+      <c r="BD9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BE9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BF9" s="2">
+        <v>16000</v>
+      </c>
+      <c r="BG9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BH9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="BI9" s="2">
+        <v>16000</v>
+      </c>
+      <c r="BJ9" s="2">
+        <v>16000</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>6000</v>
@@ -1848,13 +2581,82 @@
       <c r="AM10" s="2">
         <v>9000</v>
       </c>
+      <c r="AN10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AQ10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AR10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AS10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AT10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AU10" s="2">
+        <v>9000</v>
+      </c>
+      <c r="AV10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="AW10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AX10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AY10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AZ10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="BA10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BB10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BC10" s="2">
+        <v>9000</v>
+      </c>
+      <c r="BD10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BE10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BF10" s="2">
+        <v>9000</v>
+      </c>
+      <c r="BG10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BH10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BI10" s="2">
+        <v>9000</v>
+      </c>
+      <c r="BJ10" s="2">
+        <v>9000</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2">
         <v>1000</v>
@@ -1967,13 +2769,82 @@
       <c r="AM11" s="2">
         <v>3000</v>
       </c>
+      <c r="AN11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AQ11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AR11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AS11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AT11" s="2">
+        <v>4000</v>
+      </c>
+      <c r="AU11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AV11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AW11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AX11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AY11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AZ11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BA11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BB11" s="2">
+        <v>4000</v>
+      </c>
+      <c r="BC11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BD11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BE11" s="2">
+        <v>4000</v>
+      </c>
+      <c r="BF11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BG11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BH11" s="2">
+        <v>4000</v>
+      </c>
+      <c r="BI11" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BJ11" s="2">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
         <v>2500</v>
@@ -2086,13 +2957,82 @@
       <c r="AM12" s="2">
         <v>12000</v>
       </c>
+      <c r="AN12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AP12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AQ12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AR12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AS12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="AT12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="AU12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="AV12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AW12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AX12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AY12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AZ12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="BA12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BB12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BC12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BD12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BE12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BF12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BG12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BH12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BI12" s="2">
+        <v>12000</v>
+      </c>
+      <c r="BJ12" s="2">
+        <v>12000</v>
+      </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2">
         <v>500</v>
@@ -2205,8 +3145,77 @@
       <c r="AM13" s="2">
         <v>1500</v>
       </c>
+      <c r="AN13" s="2">
+        <v>500</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AP13" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AS13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AT13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AV13" s="2">
+        <v>500</v>
+      </c>
+      <c r="AW13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AX13" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AY13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="AZ13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BB13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BD13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BE13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BF13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BG13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BH13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BI13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>1500</v>
+      </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2322,6 +3331,75 @@
         <v>3000</v>
       </c>
       <c r="AM14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AR14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AT14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AU14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AV14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="AX14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AY14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="AZ14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BA14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BB14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BC14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BD14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BE14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BF14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BG14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="BH14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BI14" s="2">
+        <v>3000</v>
+      </c>
+      <c r="BJ14" s="2">
         <v>3000</v>
       </c>
     </row>

</xml_diff>